<commit_message>
getInfoMes, delDatabyFileID, checkColumn, NewTemp
</commit_message>
<xml_diff>
--- a/api/templates/shopper.xlsx
+++ b/api/templates/shopper.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\PROYECTS\BDF_SOP\S-OP_BDF\api\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94176561-387F-40EE-911D-9A23FC232B72}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7970237-EAF3-4A76-9A5F-F65FFEB492D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12135" yWindow="7200" windowWidth="18810" windowHeight="11070" xr2:uid="{B96385CE-A149-4059-AF89-DD6B5EDE4BC9}"/>
+    <workbookView xWindow="12885" yWindow="6825" windowWidth="15900" windowHeight="5835" xr2:uid="{B96385CE-A149-4059-AF89-DD6B5EDE4BC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -38,13 +38,7 @@
     <t>CLASIFICACION</t>
   </si>
   <si>
-    <t>TIPO DE PROMO</t>
-  </si>
-  <si>
     <t>CANAL</t>
-  </si>
-  <si>
-    <t>APPLICATION FORM</t>
   </si>
   <si>
     <t>NART</t>
@@ -54,6 +48,12 @@
   </si>
   <si>
     <t>PROMO</t>
+  </si>
+  <si>
+    <t>TIPO_PROMO</t>
+  </si>
+  <si>
+    <t>APPLICATION_FORM</t>
   </si>
 </sst>
 </file>
@@ -435,24 +435,24 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -465,18 +465,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -612,6 +612,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D77624B-4D4F-4AB2-881C-AD25FA2C8A5B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C2FF156D-FF27-4EFF-80A2-B4C4E824DC39}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
@@ -623,14 +631,6 @@
     <ds:schemaRef ds:uri="7faab0a5-b3db-4b35-b441-503bdf27f599"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D77624B-4D4F-4AB2-881C-AD25FA2C8A5B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>